<commit_message>
Added one eligible paper more
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="573">
   <si>
     <t>p.id</t>
   </si>
@@ -1720,13 +1720,28 @@
   </si>
   <si>
     <t>Mutiple social media sources (Flickr; Panoramio; Picasa Web; Geograph)</t>
+  </si>
+  <si>
+    <t>p82</t>
+  </si>
+  <si>
+    <t>Location privacy models in mobile applications: conceptual view and research directions</t>
+  </si>
+  <si>
+    <t>Geoinformatica</t>
+  </si>
+  <si>
+    <t>location privacy; location privacy metrics; location-aware applications</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.1007/s10707-014-0205-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1753,14 +1768,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1790,14 +1797,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2105,10 +2115,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P91" sqref="P91"/>
+      <selection pane="bottomLeft" activeCell="O94" sqref="O94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8196,9 +8206,61 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="L94" s="6"/>
-      <c r="M94" s="6"/>
+    <row r="94" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>568</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C94">
+        <v>2014</v>
+      </c>
+      <c r="D94" t="s">
+        <v>570</v>
+      </c>
+      <c r="E94" t="s">
+        <v>544</v>
+      </c>
+      <c r="F94" t="s">
+        <v>571</v>
+      </c>
+      <c r="G94" t="s">
+        <v>572</v>
+      </c>
+      <c r="H94" t="s">
+        <v>55</v>
+      </c>
+      <c r="J94" t="s">
+        <v>547</v>
+      </c>
+      <c r="K94" t="s">
+        <v>301</v>
+      </c>
+      <c r="L94" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="M94" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N94" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O94" t="s">
+        <v>79</v>
+      </c>
+      <c r="P94" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>79</v>
+      </c>
+      <c r="R94" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC94" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>